<commit_message>
Changed endpoints to reflect months back
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mitprod-my.sharepoint.com/personal/eseeyave_mit_edu/Documents/git/CapHackBackend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_946C2C74D5885151B68BFDF4D80D98224E0CF323" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{AD9332E9-857D-5645-B7AD-4766F5B7772E}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="11_946C2C74D5885151B68BFDF4D80D98224E0CF323" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{6F3FECC5-8CDB-C143-A2A0-D5EFD2C088E2}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -112,12 +112,6 @@
     <t>December</t>
   </si>
   <si>
-    <t>YEAR 1</t>
-  </si>
-  <si>
-    <t>YEAR 2</t>
-  </si>
-  <si>
     <t>Day Job</t>
   </si>
   <si>
@@ -182,6 +176,12 @@
   </si>
   <si>
     <t>Jon Doe</t>
+  </si>
+  <si>
+    <t>Year 2</t>
+  </si>
+  <si>
+    <t>Year 1</t>
   </si>
 </sst>
 </file>
@@ -191,7 +191,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -237,6 +237,13 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -252,7 +259,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -269,11 +276,51 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -288,6 +335,18 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -506,13 +565,16 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AA49"/>
+  <dimension ref="A1:Z49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="H8" workbookViewId="0">
+      <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="24.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
@@ -521,7 +583,7 @@
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -590,20 +652,27 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="19" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B18" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="N18" s="15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="6" t="s">
         <v>16</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N19" s="16"/>
+    </row>
+    <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" s="1" t="s">
         <v>18</v>
       </c>
@@ -640,52 +709,47 @@
       <c r="M20" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="N20" s="3" t="s">
+      <c r="N20" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="R20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="U20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="V20" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="W20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="X20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z20" s="3"/>
+    </row>
+    <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="O20" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="P20" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q20" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="R20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="S20" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="T20" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="U20" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="V20" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="W20" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="X20" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y20" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="Z20" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA20" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="21" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="B21" s="7">
         <v>600</v>
@@ -723,54 +787,47 @@
       <c r="M21" s="7">
         <v>600</v>
       </c>
-      <c r="N21" s="8">
-        <f t="shared" ref="N21:N24" si="0">SUM(B21:M21)</f>
-        <v>7200</v>
+      <c r="N21" s="18">
+        <v>600</v>
       </c>
       <c r="O21" s="7">
-        <v>600</v>
+        <v>575</v>
       </c>
       <c r="P21" s="7">
+        <v>450</v>
+      </c>
+      <c r="Q21" s="7">
+        <v>0</v>
+      </c>
+      <c r="R21" s="7">
+        <v>225</v>
+      </c>
+      <c r="S21" s="7">
+        <v>380</v>
+      </c>
+      <c r="T21" s="7">
+        <v>500</v>
+      </c>
+      <c r="U21" s="7">
+        <v>550</v>
+      </c>
+      <c r="V21" s="7">
         <v>575</v>
       </c>
-      <c r="Q21" s="7">
-        <v>450</v>
-      </c>
-      <c r="R21" s="7">
-        <v>0</v>
-      </c>
-      <c r="S21" s="7">
-        <v>225</v>
-      </c>
-      <c r="T21" s="7">
-        <v>380</v>
-      </c>
-      <c r="U21" s="7">
-        <v>500</v>
-      </c>
-      <c r="V21" s="7">
-        <v>550</v>
-      </c>
       <c r="W21" s="7">
-        <v>575</v>
+        <v>580</v>
       </c>
       <c r="X21" s="7">
         <v>580</v>
       </c>
       <c r="Y21" s="7">
-        <v>580</v>
-      </c>
-      <c r="Z21" s="7">
         <v>570</v>
       </c>
-      <c r="AA21" s="8">
-        <f t="shared" ref="AA21:AA24" si="1">SUM(O21:Z21)</f>
-        <v>5585</v>
-      </c>
-    </row>
-    <row r="22" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="Z21" s="8"/>
+    </row>
+    <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B22" s="7">
         <v>50</v>
@@ -808,253 +865,242 @@
       <c r="M22" s="7">
         <v>120</v>
       </c>
-      <c r="N22" s="8">
+      <c r="N22" s="18">
+        <v>175</v>
+      </c>
+      <c r="O22" s="7">
+        <v>220</v>
+      </c>
+      <c r="P22" s="7">
+        <v>210</v>
+      </c>
+      <c r="Q22" s="7">
+        <v>130</v>
+      </c>
+      <c r="R22" s="7">
+        <v>170</v>
+      </c>
+      <c r="S22" s="7">
+        <v>150</v>
+      </c>
+      <c r="T22" s="7">
+        <v>180</v>
+      </c>
+      <c r="U22" s="7">
+        <v>190</v>
+      </c>
+      <c r="V22" s="7">
+        <v>90</v>
+      </c>
+      <c r="W22" s="7">
+        <v>70</v>
+      </c>
+      <c r="X22" s="7">
+        <v>150</v>
+      </c>
+      <c r="Y22" s="7">
+        <v>170</v>
+      </c>
+      <c r="Z22" s="8"/>
+    </row>
+    <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" s="23">
+        <v>12</v>
+      </c>
+      <c r="C23" s="23">
+        <v>13</v>
+      </c>
+      <c r="D23" s="23">
+        <v>12</v>
+      </c>
+      <c r="E23" s="23">
+        <v>15</v>
+      </c>
+      <c r="F23" s="23">
+        <v>17</v>
+      </c>
+      <c r="G23" s="23">
+        <v>19</v>
+      </c>
+      <c r="H23" s="23">
+        <v>21</v>
+      </c>
+      <c r="I23" s="23">
+        <v>27</v>
+      </c>
+      <c r="J23" s="23">
+        <v>24</v>
+      </c>
+      <c r="K23" s="23">
+        <v>21</v>
+      </c>
+      <c r="L23" s="23">
+        <v>23</v>
+      </c>
+      <c r="M23" s="23">
+        <v>26</v>
+      </c>
+      <c r="N23" s="24">
+        <v>14</v>
+      </c>
+      <c r="O23" s="23">
+        <v>13</v>
+      </c>
+      <c r="P23" s="23">
+        <v>41</v>
+      </c>
+      <c r="Q23" s="23">
+        <v>31</v>
+      </c>
+      <c r="R23" s="23">
+        <v>17</v>
+      </c>
+      <c r="S23" s="23">
+        <v>23</v>
+      </c>
+      <c r="T23" s="23">
+        <v>24</v>
+      </c>
+      <c r="U23" s="23">
+        <v>32</v>
+      </c>
+      <c r="V23" s="23">
+        <v>24</v>
+      </c>
+      <c r="W23" s="23">
+        <v>21</v>
+      </c>
+      <c r="X23" s="23">
+        <v>23</v>
+      </c>
+      <c r="Y23" s="23">
+        <v>32</v>
+      </c>
+      <c r="Z23" s="25"/>
+    </row>
+    <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" s="8">
+        <f t="shared" ref="B24:M24" si="0">SUM(B21:B23)</f>
+        <v>662</v>
+      </c>
+      <c r="C24" s="8">
         <f t="shared" si="0"/>
-        <v>615</v>
-      </c>
-      <c r="O22" s="7">
-        <v>175</v>
-      </c>
-      <c r="P22" s="7">
-        <v>220</v>
-      </c>
-      <c r="Q22" s="7">
-        <v>210</v>
-      </c>
-      <c r="R22" s="7">
-        <v>130</v>
-      </c>
-      <c r="S22" s="7">
-        <v>170</v>
-      </c>
-      <c r="T22" s="7">
-        <v>150</v>
-      </c>
-      <c r="U22" s="7">
-        <v>180</v>
-      </c>
-      <c r="V22" s="7">
-        <v>190</v>
-      </c>
-      <c r="W22" s="7">
-        <v>90</v>
-      </c>
-      <c r="X22" s="7">
-        <v>70</v>
-      </c>
-      <c r="Y22" s="7">
-        <v>150</v>
-      </c>
-      <c r="Z22" s="7">
-        <v>170</v>
-      </c>
-      <c r="AA22" s="8">
+        <v>658</v>
+      </c>
+      <c r="D24" s="8">
+        <f t="shared" si="0"/>
+        <v>646</v>
+      </c>
+      <c r="E24" s="8">
+        <f t="shared" si="0"/>
+        <v>655</v>
+      </c>
+      <c r="F24" s="8">
+        <f t="shared" si="0"/>
+        <v>662</v>
+      </c>
+      <c r="G24" s="8">
+        <f t="shared" si="0"/>
+        <v>651</v>
+      </c>
+      <c r="H24" s="8">
+        <f t="shared" si="0"/>
+        <v>651</v>
+      </c>
+      <c r="I24" s="8">
+        <f t="shared" si="0"/>
+        <v>662</v>
+      </c>
+      <c r="J24" s="8">
+        <f t="shared" si="0"/>
+        <v>666</v>
+      </c>
+      <c r="K24" s="8">
+        <f t="shared" si="0"/>
+        <v>653</v>
+      </c>
+      <c r="L24" s="8">
+        <f t="shared" si="0"/>
+        <v>733</v>
+      </c>
+      <c r="M24" s="8">
+        <f t="shared" si="0"/>
+        <v>746</v>
+      </c>
+      <c r="N24" s="19">
+        <f t="shared" ref="N24:Y24" si="1">SUM(N21:N23)</f>
+        <v>789</v>
+      </c>
+      <c r="O24" s="8">
         <f t="shared" si="1"/>
-        <v>1905</v>
-      </c>
-    </row>
-    <row r="23" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="1" t="s">
+        <v>808</v>
+      </c>
+      <c r="P24" s="8">
+        <f t="shared" si="1"/>
+        <v>701</v>
+      </c>
+      <c r="Q24" s="8">
+        <f t="shared" si="1"/>
+        <v>161</v>
+      </c>
+      <c r="R24" s="8">
+        <f t="shared" si="1"/>
+        <v>412</v>
+      </c>
+      <c r="S24" s="8">
+        <f t="shared" si="1"/>
+        <v>553</v>
+      </c>
+      <c r="T24" s="8">
+        <f t="shared" si="1"/>
+        <v>704</v>
+      </c>
+      <c r="U24" s="8">
+        <f t="shared" si="1"/>
+        <v>772</v>
+      </c>
+      <c r="V24" s="8">
+        <f t="shared" si="1"/>
+        <v>689</v>
+      </c>
+      <c r="W24" s="8">
+        <f t="shared" si="1"/>
+        <v>671</v>
+      </c>
+      <c r="X24" s="8">
+        <f t="shared" si="1"/>
+        <v>753</v>
+      </c>
+      <c r="Y24" s="8">
+        <f t="shared" si="1"/>
+        <v>772</v>
+      </c>
+      <c r="Z24" s="8"/>
+    </row>
+    <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N25" s="16"/>
+    </row>
+    <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N26" s="16"/>
+    </row>
+    <row r="27" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="7">
-        <v>12</v>
-      </c>
-      <c r="C23" s="7">
-        <v>13</v>
-      </c>
-      <c r="D23" s="7">
-        <v>12</v>
-      </c>
-      <c r="E23" s="7">
-        <v>15</v>
-      </c>
-      <c r="F23" s="7">
-        <v>17</v>
-      </c>
-      <c r="G23" s="7">
-        <v>19</v>
-      </c>
-      <c r="H23" s="7">
-        <v>21</v>
-      </c>
-      <c r="I23" s="7">
-        <v>27</v>
-      </c>
-      <c r="J23" s="7">
-        <v>24</v>
-      </c>
-      <c r="K23" s="7">
-        <v>21</v>
-      </c>
-      <c r="L23" s="7">
-        <v>23</v>
-      </c>
-      <c r="M23" s="7">
-        <v>26</v>
-      </c>
-      <c r="N23" s="8">
-        <f t="shared" si="0"/>
-        <v>230</v>
-      </c>
-      <c r="O23" s="7">
-        <v>14</v>
-      </c>
-      <c r="P23" s="7">
-        <v>13</v>
-      </c>
-      <c r="Q23" s="7">
-        <v>41</v>
-      </c>
-      <c r="R23" s="7">
-        <v>31</v>
-      </c>
-      <c r="S23" s="7">
-        <v>17</v>
-      </c>
-      <c r="T23" s="7">
-        <v>23</v>
-      </c>
-      <c r="U23" s="7">
-        <v>24</v>
-      </c>
-      <c r="V23" s="7">
-        <v>32</v>
-      </c>
-      <c r="W23" s="7">
-        <v>24</v>
-      </c>
-      <c r="X23" s="7">
-        <v>21</v>
-      </c>
-      <c r="Y23" s="7">
-        <v>23</v>
-      </c>
-      <c r="Z23" s="7">
-        <v>32</v>
-      </c>
-      <c r="AA23" s="8">
-        <f t="shared" si="1"/>
-        <v>295</v>
-      </c>
-    </row>
-    <row r="24" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="9" t="s">
+      <c r="N27" s="16"/>
+    </row>
+    <row r="28" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N28" s="16"/>
+    </row>
+    <row r="29" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="B24" s="8">
-        <f t="shared" ref="B24:M24" si="2">SUM(B21:B23)</f>
-        <v>662</v>
-      </c>
-      <c r="C24" s="8">
-        <f t="shared" si="2"/>
-        <v>658</v>
-      </c>
-      <c r="D24" s="8">
-        <f t="shared" si="2"/>
-        <v>646</v>
-      </c>
-      <c r="E24" s="8">
-        <f t="shared" si="2"/>
-        <v>655</v>
-      </c>
-      <c r="F24" s="8">
-        <f t="shared" si="2"/>
-        <v>662</v>
-      </c>
-      <c r="G24" s="8">
-        <f t="shared" si="2"/>
-        <v>651</v>
-      </c>
-      <c r="H24" s="8">
-        <f t="shared" si="2"/>
-        <v>651</v>
-      </c>
-      <c r="I24" s="8">
-        <f t="shared" si="2"/>
-        <v>662</v>
-      </c>
-      <c r="J24" s="8">
-        <f t="shared" si="2"/>
-        <v>666</v>
-      </c>
-      <c r="K24" s="8">
-        <f t="shared" si="2"/>
-        <v>653</v>
-      </c>
-      <c r="L24" s="8">
-        <f t="shared" si="2"/>
-        <v>733</v>
-      </c>
-      <c r="M24" s="8">
-        <f t="shared" si="2"/>
-        <v>746</v>
-      </c>
-      <c r="N24" s="8">
-        <f t="shared" si="0"/>
-        <v>8045</v>
-      </c>
-      <c r="O24" s="8">
-        <f t="shared" ref="O24:Z24" si="3">SUM(O21:O23)</f>
-        <v>789</v>
-      </c>
-      <c r="P24" s="8">
-        <f t="shared" si="3"/>
-        <v>808</v>
-      </c>
-      <c r="Q24" s="8">
-        <f t="shared" si="3"/>
-        <v>701</v>
-      </c>
-      <c r="R24" s="8">
-        <f t="shared" si="3"/>
-        <v>161</v>
-      </c>
-      <c r="S24" s="8">
-        <f t="shared" si="3"/>
-        <v>412</v>
-      </c>
-      <c r="T24" s="8">
-        <f t="shared" si="3"/>
-        <v>553</v>
-      </c>
-      <c r="U24" s="8">
-        <f t="shared" si="3"/>
-        <v>704</v>
-      </c>
-      <c r="V24" s="8">
-        <f t="shared" si="3"/>
-        <v>772</v>
-      </c>
-      <c r="W24" s="8">
-        <f t="shared" si="3"/>
-        <v>689</v>
-      </c>
-      <c r="X24" s="8">
-        <f t="shared" si="3"/>
-        <v>671</v>
-      </c>
-      <c r="Y24" s="8">
-        <f t="shared" si="3"/>
-        <v>753</v>
-      </c>
-      <c r="Z24" s="8">
-        <f t="shared" si="3"/>
-        <v>772</v>
-      </c>
-      <c r="AA24" s="8">
-        <f t="shared" si="1"/>
-        <v>7785</v>
-      </c>
-    </row>
-    <row r="27" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="29" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="B29" s="7">
         <v>280</v>
@@ -1092,54 +1138,47 @@
       <c r="M29" s="7">
         <v>350</v>
       </c>
-      <c r="N29" s="8">
-        <f t="shared" ref="N29:N31" si="4">SUM(B29:M29)</f>
-        <v>3583</v>
+      <c r="N29" s="18">
+        <v>290</v>
       </c>
       <c r="O29" s="7">
+        <v>310</v>
+      </c>
+      <c r="P29" s="7">
+        <v>330</v>
+      </c>
+      <c r="Q29" s="7">
+        <v>280</v>
+      </c>
+      <c r="R29" s="7">
+        <v>285</v>
+      </c>
+      <c r="S29" s="7">
         <v>290</v>
       </c>
-      <c r="P29" s="7">
+      <c r="T29" s="7">
+        <v>291</v>
+      </c>
+      <c r="U29" s="7">
+        <v>330</v>
+      </c>
+      <c r="V29" s="7">
         <v>310</v>
       </c>
-      <c r="Q29" s="7">
-        <v>330</v>
-      </c>
-      <c r="R29" s="7">
-        <v>280</v>
-      </c>
-      <c r="S29" s="7">
-        <v>285</v>
-      </c>
-      <c r="T29" s="7">
+      <c r="W29" s="7">
         <v>290</v>
       </c>
-      <c r="U29" s="7">
-        <v>291</v>
-      </c>
-      <c r="V29" s="7">
-        <v>330</v>
-      </c>
-      <c r="W29" s="7">
-        <v>310</v>
-      </c>
       <c r="X29" s="7">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="Y29" s="7">
-        <v>287</v>
-      </c>
-      <c r="Z29" s="7">
         <v>340</v>
       </c>
-      <c r="AA29" s="8">
-        <f t="shared" ref="AA29:AA31" si="5">SUM(O29:Z29)</f>
-        <v>3633</v>
-      </c>
-    </row>
-    <row r="30" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="Z29" s="8"/>
+    </row>
+    <row r="30" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B30" s="11">
         <v>76</v>
@@ -1177,163 +1216,152 @@
       <c r="M30" s="11">
         <v>120</v>
       </c>
-      <c r="N30" s="8">
-        <f t="shared" si="4"/>
-        <v>1397</v>
+      <c r="N30" s="20">
+        <v>140</v>
       </c>
       <c r="O30" s="11">
-        <v>140</v>
+        <v>75</v>
       </c>
       <c r="P30" s="11">
         <v>75</v>
       </c>
       <c r="Q30" s="11">
-        <v>75</v>
+        <v>170</v>
       </c>
       <c r="R30" s="11">
-        <v>170</v>
+        <v>150</v>
       </c>
       <c r="S30" s="11">
+        <v>100</v>
+      </c>
+      <c r="T30" s="11">
         <v>150</v>
       </c>
-      <c r="T30" s="11">
+      <c r="U30" s="11">
+        <v>160</v>
+      </c>
+      <c r="V30" s="11">
+        <v>120</v>
+      </c>
+      <c r="W30" s="11">
+        <v>115</v>
+      </c>
+      <c r="X30" s="11">
+        <v>112</v>
+      </c>
+      <c r="Y30" s="11">
         <v>100</v>
       </c>
-      <c r="U30" s="11">
-        <v>150</v>
-      </c>
-      <c r="V30" s="11">
-        <v>160</v>
-      </c>
-      <c r="W30" s="11">
-        <v>120</v>
-      </c>
-      <c r="X30" s="11">
-        <v>115</v>
-      </c>
-      <c r="Y30" s="11">
-        <v>112</v>
-      </c>
-      <c r="Z30" s="11">
-        <v>100</v>
-      </c>
-      <c r="AA30" s="8">
-        <f t="shared" si="5"/>
-        <v>1467</v>
-      </c>
-    </row>
-    <row r="31" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="Z30" s="8"/>
+    </row>
+    <row r="31" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B31" s="8">
-        <f t="shared" ref="B31:M31" si="6">SUM(B29:B30)</f>
+        <f t="shared" ref="B31:M31" si="2">SUM(B29:B30)</f>
         <v>356</v>
       </c>
       <c r="C31" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>375</v>
       </c>
       <c r="D31" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>359</v>
       </c>
       <c r="E31" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>440</v>
       </c>
       <c r="F31" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>435</v>
       </c>
       <c r="G31" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>380</v>
       </c>
       <c r="H31" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>475</v>
       </c>
       <c r="I31" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>460</v>
       </c>
       <c r="J31" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>370</v>
       </c>
       <c r="K31" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>401</v>
       </c>
       <c r="L31" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>459</v>
       </c>
       <c r="M31" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>470</v>
       </c>
-      <c r="N31" s="8">
-        <f t="shared" si="4"/>
-        <v>4980</v>
+      <c r="N31" s="19">
+        <f t="shared" ref="N31:Y31" si="3">SUM(N29:N30)</f>
+        <v>430</v>
       </c>
       <c r="O31" s="8">
-        <f t="shared" ref="O31:Z31" si="7">SUM(O29:O30)</f>
+        <f t="shared" si="3"/>
+        <v>385</v>
+      </c>
+      <c r="P31" s="8">
+        <f t="shared" si="3"/>
+        <v>405</v>
+      </c>
+      <c r="Q31" s="8">
+        <f t="shared" si="3"/>
+        <v>450</v>
+      </c>
+      <c r="R31" s="8">
+        <f t="shared" si="3"/>
+        <v>435</v>
+      </c>
+      <c r="S31" s="8">
+        <f t="shared" si="3"/>
+        <v>390</v>
+      </c>
+      <c r="T31" s="8">
+        <f t="shared" si="3"/>
+        <v>441</v>
+      </c>
+      <c r="U31" s="8">
+        <f t="shared" si="3"/>
+        <v>490</v>
+      </c>
+      <c r="V31" s="8">
+        <f t="shared" si="3"/>
         <v>430</v>
       </c>
-      <c r="P31" s="8">
-        <f t="shared" si="7"/>
-        <v>385</v>
-      </c>
-      <c r="Q31" s="8">
-        <f t="shared" si="7"/>
+      <c r="W31" s="8">
+        <f t="shared" si="3"/>
         <v>405</v>
       </c>
-      <c r="R31" s="8">
-        <f t="shared" si="7"/>
-        <v>450</v>
-      </c>
-      <c r="S31" s="8">
-        <f t="shared" si="7"/>
-        <v>435</v>
-      </c>
-      <c r="T31" s="8">
-        <f t="shared" si="7"/>
-        <v>390</v>
-      </c>
-      <c r="U31" s="8">
-        <f t="shared" si="7"/>
-        <v>441</v>
-      </c>
-      <c r="V31" s="8">
-        <f t="shared" si="7"/>
-        <v>490</v>
-      </c>
-      <c r="W31" s="8">
-        <f t="shared" si="7"/>
-        <v>430</v>
-      </c>
       <c r="X31" s="8">
-        <f t="shared" si="7"/>
-        <v>405</v>
+        <f t="shared" si="3"/>
+        <v>399</v>
       </c>
       <c r="Y31" s="8">
-        <f t="shared" si="7"/>
-        <v>399</v>
-      </c>
-      <c r="Z31" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>440</v>
       </c>
-      <c r="AA31" s="8">
-        <f t="shared" si="5"/>
-        <v>5100</v>
-      </c>
-    </row>
-    <row r="33" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="Z31" s="8"/>
+    </row>
+    <row r="32" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N32" s="16"/>
+    </row>
+    <row r="33" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B33" s="7">
         <v>19</v>
@@ -1371,54 +1399,47 @@
       <c r="M33" s="7">
         <v>19</v>
       </c>
-      <c r="N33" s="8">
-        <f t="shared" ref="N33:N35" si="8">SUM(B33:M33)</f>
-        <v>254</v>
+      <c r="N33" s="18">
+        <v>19</v>
       </c>
       <c r="O33" s="7">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="P33" s="7">
+        <v>20</v>
+      </c>
+      <c r="Q33" s="7">
+        <v>22</v>
+      </c>
+      <c r="R33" s="7">
         <v>21</v>
       </c>
-      <c r="Q33" s="7">
-        <v>20</v>
-      </c>
-      <c r="R33" s="7">
-        <v>22</v>
-      </c>
       <c r="S33" s="7">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="T33" s="7">
         <v>23</v>
       </c>
       <c r="U33" s="7">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="V33" s="7">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="W33" s="7">
+        <v>22</v>
+      </c>
+      <c r="X33" s="7">
+        <v>21</v>
+      </c>
+      <c r="Y33" s="7">
         <v>19</v>
       </c>
-      <c r="X33" s="7">
-        <v>22</v>
-      </c>
-      <c r="Y33" s="7">
-        <v>21</v>
-      </c>
-      <c r="Z33" s="7">
-        <v>19</v>
-      </c>
-      <c r="AA33" s="8">
-        <f t="shared" ref="AA33:AA35" si="9">SUM(O33:Z33)</f>
-        <v>254</v>
-      </c>
-    </row>
-    <row r="34" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="Z33" s="8"/>
+    </row>
+    <row r="34" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B34" s="11">
         <v>57</v>
@@ -1456,163 +1477,152 @@
       <c r="M34" s="11">
         <v>52</v>
       </c>
-      <c r="N34" s="8">
-        <f t="shared" si="8"/>
-        <v>628</v>
+      <c r="N34" s="20">
+        <v>53</v>
       </c>
       <c r="O34" s="11">
+        <v>49</v>
+      </c>
+      <c r="P34" s="11">
+        <v>51</v>
+      </c>
+      <c r="Q34" s="11">
+        <v>52</v>
+      </c>
+      <c r="R34" s="11">
+        <v>51</v>
+      </c>
+      <c r="S34" s="11">
+        <v>47</v>
+      </c>
+      <c r="T34" s="11">
+        <v>46</v>
+      </c>
+      <c r="U34" s="11">
+        <v>45</v>
+      </c>
+      <c r="V34" s="11">
+        <v>46</v>
+      </c>
+      <c r="W34" s="11">
+        <v>48</v>
+      </c>
+      <c r="X34" s="11">
+        <v>51</v>
+      </c>
+      <c r="Y34" s="11">
         <v>53</v>
       </c>
-      <c r="P34" s="11">
-        <v>49</v>
-      </c>
-      <c r="Q34" s="11">
-        <v>51</v>
-      </c>
-      <c r="R34" s="11">
-        <v>52</v>
-      </c>
-      <c r="S34" s="11">
-        <v>51</v>
-      </c>
-      <c r="T34" s="11">
-        <v>47</v>
-      </c>
-      <c r="U34" s="11">
-        <v>46</v>
-      </c>
-      <c r="V34" s="11">
-        <v>45</v>
-      </c>
-      <c r="W34" s="11">
-        <v>46</v>
-      </c>
-      <c r="X34" s="11">
-        <v>48</v>
-      </c>
-      <c r="Y34" s="11">
-        <v>51</v>
-      </c>
-      <c r="Z34" s="11">
-        <v>53</v>
-      </c>
-      <c r="AA34" s="8">
-        <f t="shared" si="9"/>
-        <v>592</v>
-      </c>
-    </row>
-    <row r="35" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="Z34" s="8"/>
+    </row>
+    <row r="35" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B35" s="8">
-        <f t="shared" ref="B35:M35" si="10">SUM(B33:B34)</f>
+        <f t="shared" ref="B35:M35" si="4">SUM(B33:B34)</f>
         <v>76</v>
       </c>
       <c r="C35" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="4"/>
         <v>74</v>
       </c>
       <c r="D35" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="4"/>
         <v>74</v>
       </c>
       <c r="E35" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="4"/>
         <v>79</v>
       </c>
       <c r="F35" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="4"/>
         <v>75</v>
       </c>
       <c r="G35" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="4"/>
         <v>73</v>
       </c>
       <c r="H35" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="4"/>
         <v>72</v>
       </c>
       <c r="I35" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="4"/>
         <v>73</v>
       </c>
       <c r="J35" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="4"/>
         <v>70</v>
       </c>
       <c r="K35" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="4"/>
         <v>70</v>
       </c>
       <c r="L35" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="4"/>
         <v>75</v>
       </c>
       <c r="M35" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="4"/>
         <v>71</v>
       </c>
-      <c r="N35" s="8">
-        <f t="shared" si="8"/>
-        <v>882</v>
+      <c r="N35" s="19">
+        <f t="shared" ref="N35:Y35" si="5">SUM(N33:N34)</f>
+        <v>72</v>
       </c>
       <c r="O35" s="8">
-        <f t="shared" ref="O35:Z35" si="11">SUM(O33:O34)</f>
+        <f t="shared" si="5"/>
+        <v>70</v>
+      </c>
+      <c r="P35" s="8">
+        <f t="shared" si="5"/>
+        <v>71</v>
+      </c>
+      <c r="Q35" s="8">
+        <f t="shared" si="5"/>
+        <v>74</v>
+      </c>
+      <c r="R35" s="8">
+        <f t="shared" si="5"/>
         <v>72</v>
       </c>
-      <c r="P35" s="8">
-        <f t="shared" si="11"/>
+      <c r="S35" s="8">
+        <f t="shared" si="5"/>
         <v>70</v>
       </c>
-      <c r="Q35" s="8">
-        <f t="shared" si="11"/>
-        <v>71</v>
-      </c>
-      <c r="R35" s="8">
-        <f t="shared" si="11"/>
-        <v>74</v>
-      </c>
-      <c r="S35" s="8">
-        <f t="shared" si="11"/>
+      <c r="T35" s="8">
+        <f t="shared" si="5"/>
+        <v>69</v>
+      </c>
+      <c r="U35" s="8">
+        <f t="shared" si="5"/>
+        <v>69</v>
+      </c>
+      <c r="V35" s="8">
+        <f t="shared" si="5"/>
+        <v>65</v>
+      </c>
+      <c r="W35" s="8">
+        <f t="shared" si="5"/>
+        <v>70</v>
+      </c>
+      <c r="X35" s="8">
+        <f t="shared" si="5"/>
         <v>72</v>
       </c>
-      <c r="T35" s="8">
-        <f t="shared" si="11"/>
-        <v>70</v>
-      </c>
-      <c r="U35" s="8">
-        <f t="shared" si="11"/>
-        <v>69</v>
-      </c>
-      <c r="V35" s="8">
-        <f t="shared" si="11"/>
-        <v>69</v>
-      </c>
-      <c r="W35" s="8">
-        <f t="shared" si="11"/>
-        <v>65</v>
-      </c>
-      <c r="X35" s="8">
-        <f t="shared" si="11"/>
-        <v>70</v>
-      </c>
       <c r="Y35" s="8">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>72</v>
       </c>
-      <c r="Z35" s="8">
-        <f t="shared" si="11"/>
-        <v>72</v>
-      </c>
-      <c r="AA35" s="8">
-        <f t="shared" si="9"/>
-        <v>846</v>
-      </c>
-    </row>
-    <row r="37" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="Z35" s="8"/>
+    </row>
+    <row r="36" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N36" s="16"/>
+    </row>
+    <row r="37" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B37" s="7">
         <v>50</v>
@@ -1650,54 +1660,47 @@
       <c r="M37" s="7">
         <v>50</v>
       </c>
-      <c r="N37" s="8">
-        <f t="shared" ref="N37:N40" si="12">SUM(B37:M37)</f>
-        <v>601</v>
+      <c r="N37" s="18">
+        <v>50</v>
       </c>
       <c r="O37" s="7">
+        <v>51</v>
+      </c>
+      <c r="P37" s="7">
+        <v>36</v>
+      </c>
+      <c r="Q37" s="7">
+        <v>0</v>
+      </c>
+      <c r="R37" s="7">
+        <v>0</v>
+      </c>
+      <c r="S37" s="7">
+        <v>0</v>
+      </c>
+      <c r="T37" s="7">
+        <v>5</v>
+      </c>
+      <c r="U37" s="7">
+        <v>10</v>
+      </c>
+      <c r="V37" s="7">
+        <v>30</v>
+      </c>
+      <c r="W37" s="7">
+        <v>35</v>
+      </c>
+      <c r="X37" s="7">
         <v>50</v>
       </c>
-      <c r="P37" s="7">
-        <v>51</v>
-      </c>
-      <c r="Q37" s="7">
-        <v>36</v>
-      </c>
-      <c r="R37" s="7">
-        <v>0</v>
-      </c>
-      <c r="S37" s="7">
-        <v>0</v>
-      </c>
-      <c r="T37" s="7">
-        <v>0</v>
-      </c>
-      <c r="U37" s="7">
-        <v>5</v>
-      </c>
-      <c r="V37" s="7">
-        <v>10</v>
-      </c>
-      <c r="W37" s="7">
-        <v>30</v>
-      </c>
-      <c r="X37" s="7">
-        <v>35</v>
-      </c>
       <c r="Y37" s="7">
-        <v>50</v>
-      </c>
-      <c r="Z37" s="7">
         <v>45</v>
       </c>
-      <c r="AA37" s="8">
-        <f t="shared" ref="AA37:AA40" si="13">SUM(O37:Z37)</f>
-        <v>312</v>
-      </c>
-    </row>
-    <row r="38" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="Z37" s="8"/>
+    </row>
+    <row r="38" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B38" s="7">
         <v>190</v>
@@ -1735,13 +1738,12 @@
       <c r="M38" s="1">
         <v>0</v>
       </c>
-      <c r="N38" s="8">
-        <f t="shared" si="12"/>
-        <v>560</v>
-      </c>
-      <c r="O38" s="7">
+      <c r="N38" s="18">
         <v>170</v>
       </c>
+      <c r="O38" s="1">
+        <v>0</v>
+      </c>
       <c r="P38" s="1">
         <v>0</v>
       </c>
@@ -1772,17 +1774,11 @@
       <c r="Y38" s="1">
         <v>0</v>
       </c>
-      <c r="Z38" s="1">
-        <v>0</v>
-      </c>
-      <c r="AA38" s="8">
-        <f t="shared" si="13"/>
-        <v>170</v>
-      </c>
-    </row>
-    <row r="39" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="Z38" s="8"/>
+    </row>
+    <row r="39" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B39" s="11">
         <v>110</v>
@@ -1820,163 +1816,152 @@
       <c r="M39" s="11">
         <v>45</v>
       </c>
-      <c r="N39" s="8">
-        <f t="shared" si="12"/>
-        <v>791</v>
+      <c r="N39" s="20">
+        <v>150</v>
       </c>
       <c r="O39" s="11">
+        <v>170</v>
+      </c>
+      <c r="P39" s="11">
+        <v>96</v>
+      </c>
+      <c r="Q39" s="10">
+        <v>0</v>
+      </c>
+      <c r="R39" s="10">
+        <v>0</v>
+      </c>
+      <c r="S39" s="11">
+        <v>40</v>
+      </c>
+      <c r="T39" s="11">
+        <v>39</v>
+      </c>
+      <c r="U39" s="11">
+        <v>50</v>
+      </c>
+      <c r="V39" s="11">
+        <v>60</v>
+      </c>
+      <c r="W39" s="11">
+        <v>70</v>
+      </c>
+      <c r="X39" s="11">
+        <v>40</v>
+      </c>
+      <c r="Y39" s="11">
+        <v>45</v>
+      </c>
+      <c r="Z39" s="8"/>
+    </row>
+    <row r="40" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A40" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B40" s="8">
+        <f t="shared" ref="B40:M40" si="6">SUM(B37:B39)</f>
+        <v>350</v>
+      </c>
+      <c r="C40" s="8">
+        <f t="shared" si="6"/>
+        <v>171</v>
+      </c>
+      <c r="D40" s="8">
+        <f t="shared" si="6"/>
+        <v>146</v>
+      </c>
+      <c r="E40" s="8">
+        <f t="shared" si="6"/>
+        <v>170</v>
+      </c>
+      <c r="F40" s="8">
+        <f t="shared" si="6"/>
         <v>150</v>
       </c>
-      <c r="P39" s="11">
-        <v>170</v>
-      </c>
-      <c r="Q39" s="11">
-        <v>96</v>
-      </c>
-      <c r="R39" s="10">
-        <v>0</v>
-      </c>
-      <c r="S39" s="10">
-        <v>0</v>
-      </c>
-      <c r="T39" s="11">
+      <c r="G40" s="8">
+        <f t="shared" si="6"/>
+        <v>160</v>
+      </c>
+      <c r="H40" s="8">
+        <f t="shared" si="6"/>
+        <v>100</v>
+      </c>
+      <c r="I40" s="8">
+        <f t="shared" si="6"/>
+        <v>100</v>
+      </c>
+      <c r="J40" s="8">
+        <f t="shared" si="6"/>
+        <v>110</v>
+      </c>
+      <c r="K40" s="8">
+        <f t="shared" si="6"/>
+        <v>160</v>
+      </c>
+      <c r="L40" s="8">
+        <f t="shared" si="6"/>
+        <v>240</v>
+      </c>
+      <c r="M40" s="8">
+        <f t="shared" si="6"/>
+        <v>95</v>
+      </c>
+      <c r="N40" s="19">
+        <f t="shared" ref="N40:Y40" si="7">SUM(N37:N39)</f>
+        <v>370</v>
+      </c>
+      <c r="O40" s="8">
+        <f t="shared" si="7"/>
+        <v>221</v>
+      </c>
+      <c r="P40" s="8">
+        <f t="shared" si="7"/>
+        <v>132</v>
+      </c>
+      <c r="Q40" s="8">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="R40" s="8">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S40" s="8">
+        <f t="shared" si="7"/>
         <v>40</v>
       </c>
-      <c r="U39" s="11">
-        <v>39</v>
-      </c>
-      <c r="V39" s="11">
-        <v>50</v>
-      </c>
-      <c r="W39" s="11">
+      <c r="T40" s="8">
+        <f t="shared" si="7"/>
+        <v>44</v>
+      </c>
+      <c r="U40" s="8">
+        <f t="shared" si="7"/>
         <v>60</v>
       </c>
-      <c r="X39" s="11">
-        <v>70</v>
-      </c>
-      <c r="Y39" s="11">
-        <v>40</v>
-      </c>
-      <c r="Z39" s="11">
+      <c r="V40" s="8">
+        <f t="shared" si="7"/>
+        <v>90</v>
+      </c>
+      <c r="W40" s="8">
+        <f t="shared" si="7"/>
+        <v>105</v>
+      </c>
+      <c r="X40" s="8">
+        <f t="shared" si="7"/>
+        <v>90</v>
+      </c>
+      <c r="Y40" s="8">
+        <f t="shared" si="7"/>
+        <v>90</v>
+      </c>
+      <c r="Z40" s="8"/>
+    </row>
+    <row r="41" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N41" s="16"/>
+    </row>
+    <row r="42" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A42" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="AA39" s="8">
-        <f t="shared" si="13"/>
-        <v>760</v>
-      </c>
-    </row>
-    <row r="40" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A40" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="B40" s="8">
-        <f t="shared" ref="B40:M40" si="14">SUM(B37:B39)</f>
-        <v>350</v>
-      </c>
-      <c r="C40" s="8">
-        <f t="shared" si="14"/>
-        <v>171</v>
-      </c>
-      <c r="D40" s="8">
-        <f t="shared" si="14"/>
-        <v>146</v>
-      </c>
-      <c r="E40" s="8">
-        <f t="shared" si="14"/>
-        <v>170</v>
-      </c>
-      <c r="F40" s="8">
-        <f t="shared" si="14"/>
-        <v>150</v>
-      </c>
-      <c r="G40" s="8">
-        <f t="shared" si="14"/>
-        <v>160</v>
-      </c>
-      <c r="H40" s="8">
-        <f t="shared" si="14"/>
-        <v>100</v>
-      </c>
-      <c r="I40" s="8">
-        <f t="shared" si="14"/>
-        <v>100</v>
-      </c>
-      <c r="J40" s="8">
-        <f t="shared" si="14"/>
-        <v>110</v>
-      </c>
-      <c r="K40" s="8">
-        <f t="shared" si="14"/>
-        <v>160</v>
-      </c>
-      <c r="L40" s="8">
-        <f t="shared" si="14"/>
-        <v>240</v>
-      </c>
-      <c r="M40" s="8">
-        <f t="shared" si="14"/>
-        <v>95</v>
-      </c>
-      <c r="N40" s="8">
-        <f t="shared" si="12"/>
-        <v>1952</v>
-      </c>
-      <c r="O40" s="8">
-        <f t="shared" ref="O40:Z40" si="15">SUM(O37:O39)</f>
-        <v>370</v>
-      </c>
-      <c r="P40" s="8">
-        <f t="shared" si="15"/>
-        <v>221</v>
-      </c>
-      <c r="Q40" s="8">
-        <f t="shared" si="15"/>
-        <v>132</v>
-      </c>
-      <c r="R40" s="8">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="S40" s="8">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="T40" s="8">
-        <f t="shared" si="15"/>
-        <v>40</v>
-      </c>
-      <c r="U40" s="8">
-        <f t="shared" si="15"/>
-        <v>44</v>
-      </c>
-      <c r="V40" s="8">
-        <f t="shared" si="15"/>
-        <v>60</v>
-      </c>
-      <c r="W40" s="8">
-        <f t="shared" si="15"/>
-        <v>90</v>
-      </c>
-      <c r="X40" s="8">
-        <f t="shared" si="15"/>
-        <v>105</v>
-      </c>
-      <c r="Y40" s="8">
-        <f t="shared" si="15"/>
-        <v>90</v>
-      </c>
-      <c r="Z40" s="8">
-        <f t="shared" si="15"/>
-        <v>90</v>
-      </c>
-      <c r="AA40" s="8">
-        <f t="shared" si="13"/>
-        <v>1242</v>
-      </c>
-    </row>
-    <row r="42" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="B42" s="7">
         <v>13</v>
@@ -2014,9 +1999,8 @@
       <c r="M42" s="7">
         <v>13</v>
       </c>
-      <c r="N42" s="8">
-        <f t="shared" ref="N42:N45" si="16">SUM(B42:M42)</f>
-        <v>156</v>
+      <c r="N42" s="18">
+        <v>15</v>
       </c>
       <c r="O42" s="7">
         <v>15</v>
@@ -2051,17 +2035,11 @@
       <c r="Y42" s="7">
         <v>15</v>
       </c>
-      <c r="Z42" s="7">
-        <v>15</v>
-      </c>
-      <c r="AA42" s="8">
-        <f t="shared" ref="AA42:AA45" si="17">SUM(O42:Z42)</f>
-        <v>180</v>
-      </c>
-    </row>
-    <row r="43" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="Z42" s="8"/>
+    </row>
+    <row r="43" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B43" s="7">
         <v>10</v>
@@ -2099,9 +2077,8 @@
       <c r="M43" s="7">
         <v>10</v>
       </c>
-      <c r="N43" s="8">
-        <f t="shared" si="16"/>
-        <v>120</v>
+      <c r="N43" s="18">
+        <v>10</v>
       </c>
       <c r="O43" s="7">
         <v>10</v>
@@ -2136,17 +2113,11 @@
       <c r="Y43" s="7">
         <v>10</v>
       </c>
-      <c r="Z43" s="7">
-        <v>10</v>
-      </c>
-      <c r="AA43" s="8">
-        <f t="shared" si="17"/>
-        <v>120</v>
-      </c>
-    </row>
-    <row r="44" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="Z43" s="8"/>
+    </row>
+    <row r="44" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B44" s="11">
         <v>34</v>
@@ -2184,9 +2155,8 @@
       <c r="M44" s="11">
         <v>34</v>
       </c>
-      <c r="N44" s="8">
-        <f t="shared" si="16"/>
-        <v>408</v>
+      <c r="N44" s="20">
+        <v>34</v>
       </c>
       <c r="O44" s="11">
         <v>34</v>
@@ -2221,126 +2191,116 @@
       <c r="Y44" s="11">
         <v>34</v>
       </c>
-      <c r="Z44" s="11">
-        <v>34</v>
-      </c>
-      <c r="AA44" s="8">
-        <f t="shared" si="17"/>
-        <v>408</v>
-      </c>
-    </row>
-    <row r="45" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="Z44" s="8"/>
+    </row>
+    <row r="45" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B45" s="8">
-        <f t="shared" ref="B45:M45" si="18">SUM(B42:B44)</f>
+        <f t="shared" ref="B45:M45" si="8">SUM(B42:B44)</f>
         <v>57</v>
       </c>
       <c r="C45" s="8">
-        <f t="shared" si="18"/>
+        <f t="shared" si="8"/>
         <v>57</v>
       </c>
       <c r="D45" s="8">
-        <f t="shared" si="18"/>
+        <f t="shared" si="8"/>
         <v>57</v>
       </c>
       <c r="E45" s="8">
-        <f t="shared" si="18"/>
+        <f t="shared" si="8"/>
         <v>57</v>
       </c>
       <c r="F45" s="8">
-        <f t="shared" si="18"/>
+        <f t="shared" si="8"/>
         <v>57</v>
       </c>
       <c r="G45" s="8">
-        <f t="shared" si="18"/>
+        <f t="shared" si="8"/>
         <v>57</v>
       </c>
       <c r="H45" s="8">
-        <f t="shared" si="18"/>
+        <f t="shared" si="8"/>
         <v>57</v>
       </c>
       <c r="I45" s="8">
-        <f t="shared" si="18"/>
+        <f t="shared" si="8"/>
         <v>57</v>
       </c>
       <c r="J45" s="8">
-        <f t="shared" si="18"/>
+        <f t="shared" si="8"/>
         <v>57</v>
       </c>
       <c r="K45" s="8">
-        <f t="shared" si="18"/>
+        <f t="shared" si="8"/>
         <v>57</v>
       </c>
       <c r="L45" s="8">
-        <f t="shared" si="18"/>
+        <f t="shared" si="8"/>
         <v>57</v>
       </c>
       <c r="M45" s="8">
-        <f t="shared" si="18"/>
+        <f t="shared" si="8"/>
         <v>57</v>
       </c>
-      <c r="N45" s="8">
-        <f t="shared" si="16"/>
-        <v>684</v>
+      <c r="N45" s="19">
+        <f t="shared" ref="N45:Y45" si="9">SUM(N42:N44)</f>
+        <v>59</v>
       </c>
       <c r="O45" s="8">
-        <f t="shared" ref="O45:Z45" si="19">SUM(O42:O44)</f>
+        <f t="shared" si="9"/>
         <v>59</v>
       </c>
       <c r="P45" s="8">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>59</v>
       </c>
       <c r="Q45" s="8">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>59</v>
       </c>
       <c r="R45" s="8">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>59</v>
       </c>
       <c r="S45" s="8">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>59</v>
       </c>
       <c r="T45" s="8">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>59</v>
       </c>
       <c r="U45" s="8">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>59</v>
       </c>
       <c r="V45" s="8">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>59</v>
       </c>
       <c r="W45" s="8">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>59</v>
       </c>
       <c r="X45" s="8">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>59</v>
       </c>
       <c r="Y45" s="8">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>59</v>
       </c>
-      <c r="Z45" s="8">
-        <f t="shared" si="19"/>
-        <v>59</v>
-      </c>
-      <c r="AA45" s="8">
-        <f t="shared" si="17"/>
-        <v>708</v>
-      </c>
-    </row>
-    <row r="47" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="Z45" s="8"/>
+    </row>
+    <row r="46" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N46" s="16"/>
+    </row>
+    <row r="47" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B47" s="7">
         <v>45</v>
@@ -2378,52 +2338,45 @@
       <c r="M47" s="7">
         <v>70</v>
       </c>
-      <c r="N47" s="8">
-        <f>SUM(B47:M47)</f>
-        <v>531</v>
+      <c r="N47" s="18">
+        <v>15</v>
       </c>
       <c r="O47" s="7">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="P47" s="7">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="Q47" s="7">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="R47" s="7">
+        <v>32</v>
+      </c>
+      <c r="S47" s="7">
+        <v>21</v>
+      </c>
+      <c r="T47" s="7">
+        <v>0</v>
+      </c>
+      <c r="U47" s="7">
+        <v>5</v>
+      </c>
+      <c r="V47" s="7">
         <v>45</v>
       </c>
-      <c r="S47" s="7">
+      <c r="W47" s="7">
         <v>32</v>
       </c>
-      <c r="T47" s="7">
-        <v>21</v>
-      </c>
-      <c r="U47" s="7">
-        <v>0</v>
-      </c>
-      <c r="V47" s="7">
-        <v>5</v>
-      </c>
-      <c r="W47" s="7">
-        <v>45</v>
-      </c>
       <c r="X47" s="7">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="Y47" s="7">
-        <v>23</v>
-      </c>
-      <c r="Z47" s="7">
         <v>70</v>
       </c>
-      <c r="AA47" s="8">
-        <f>SUM(O47:Z47)</f>
-        <v>331</v>
-      </c>
-    </row>
-    <row r="48" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="Z47" s="8"/>
+    </row>
+    <row r="48" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="13"/>
       <c r="B48" s="13"/>
       <c r="C48" s="13"/>
@@ -2437,6 +2390,7 @@
       <c r="K48" s="13"/>
       <c r="L48" s="13"/>
       <c r="M48" s="13"/>
+      <c r="N48" s="21"/>
       <c r="O48" s="13"/>
       <c r="P48" s="13"/>
       <c r="Q48" s="13"/>
@@ -2448,116 +2402,108 @@
       <c r="W48" s="13"/>
       <c r="X48" s="13"/>
       <c r="Y48" s="13"/>
-      <c r="Z48" s="13"/>
-    </row>
-    <row r="49" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="49" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B49" s="8">
-        <f t="shared" ref="B49:M49" si="20">SUM(B47,B45,B40,B35,B31)</f>
+        <f t="shared" ref="B49:M49" si="10">SUM(B47,B45,B40,B35,B31)</f>
         <v>884</v>
       </c>
       <c r="C49" s="8">
-        <f t="shared" si="20"/>
+        <f t="shared" si="10"/>
         <v>714</v>
       </c>
       <c r="D49" s="8">
-        <f t="shared" si="20"/>
+        <f t="shared" si="10"/>
         <v>692</v>
       </c>
       <c r="E49" s="8">
-        <f t="shared" si="20"/>
+        <f t="shared" si="10"/>
         <v>791</v>
       </c>
       <c r="F49" s="8">
-        <f t="shared" si="20"/>
+        <f t="shared" si="10"/>
         <v>749</v>
       </c>
       <c r="G49" s="8">
-        <f t="shared" si="20"/>
+        <f t="shared" si="10"/>
         <v>691</v>
       </c>
       <c r="H49" s="8">
-        <f t="shared" si="20"/>
+        <f t="shared" si="10"/>
         <v>719</v>
       </c>
       <c r="I49" s="8">
-        <f t="shared" si="20"/>
+        <f t="shared" si="10"/>
         <v>700</v>
       </c>
       <c r="J49" s="8">
-        <f t="shared" si="20"/>
+        <f t="shared" si="10"/>
         <v>652</v>
       </c>
       <c r="K49" s="8">
-        <f t="shared" si="20"/>
+        <f t="shared" si="10"/>
         <v>720</v>
       </c>
       <c r="L49" s="8">
-        <f t="shared" si="20"/>
+        <f t="shared" si="10"/>
         <v>954</v>
       </c>
       <c r="M49" s="8">
-        <f t="shared" si="20"/>
+        <f t="shared" si="10"/>
         <v>763</v>
       </c>
-      <c r="N49" s="8">
-        <f>SUM(B49:M49)</f>
-        <v>9029</v>
+      <c r="N49" s="19">
+        <f t="shared" ref="N49:Y49" si="11">SUM(N47,N45,N40,N35,N31)</f>
+        <v>946</v>
       </c>
       <c r="O49" s="8">
-        <f t="shared" ref="O49:Z49" si="21">SUM(O47,O45,O40,O35,O31)</f>
-        <v>946</v>
+        <f t="shared" si="11"/>
+        <v>748</v>
       </c>
       <c r="P49" s="8">
-        <f t="shared" si="21"/>
-        <v>748</v>
+        <f t="shared" si="11"/>
+        <v>697</v>
       </c>
       <c r="Q49" s="8">
-        <f t="shared" si="21"/>
-        <v>697</v>
+        <f t="shared" si="11"/>
+        <v>628</v>
       </c>
       <c r="R49" s="8">
-        <f t="shared" si="21"/>
-        <v>628</v>
+        <f t="shared" si="11"/>
+        <v>598</v>
       </c>
       <c r="S49" s="8">
-        <f t="shared" si="21"/>
-        <v>598</v>
+        <f t="shared" si="11"/>
+        <v>580</v>
       </c>
       <c r="T49" s="8">
-        <f t="shared" si="21"/>
-        <v>580</v>
+        <f t="shared" si="11"/>
+        <v>613</v>
       </c>
       <c r="U49" s="8">
-        <f t="shared" si="21"/>
-        <v>613</v>
+        <f t="shared" si="11"/>
+        <v>683</v>
       </c>
       <c r="V49" s="8">
-        <f t="shared" si="21"/>
-        <v>683</v>
+        <f t="shared" si="11"/>
+        <v>689</v>
       </c>
       <c r="W49" s="8">
-        <f t="shared" si="21"/>
-        <v>689</v>
+        <f t="shared" si="11"/>
+        <v>671</v>
       </c>
       <c r="X49" s="8">
-        <f t="shared" si="21"/>
-        <v>671</v>
+        <f t="shared" si="11"/>
+        <v>643</v>
       </c>
       <c r="Y49" s="8">
-        <f t="shared" si="21"/>
-        <v>643</v>
-      </c>
-      <c r="Z49" s="8">
-        <f t="shared" si="21"/>
+        <f t="shared" si="11"/>
         <v>731</v>
       </c>
-      <c r="AA49" s="8">
-        <f>SUM(O49:Z49)</f>
-        <v>8227</v>
-      </c>
+      <c r="Z49" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>